<commit_message>
Updates to locations and masterlists
</commit_message>
<xml_diff>
--- a/LOCATION SHEETS/1840sLOCATIONS.xlsx
+++ b/LOCATION SHEETS/1840sLOCATIONS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ed/Documents/WR4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ed/Documents/GitHub/rainfall-rescue/LOCATION SHEETS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA60333C-D581-0249-A14B-4EF5560F57B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D413F21-AFE2-FB4A-BF7C-785D686D8AB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="460" windowWidth="28100" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2200" yWindow="460" windowWidth="22520" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1840sLOCATIONS" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2232" uniqueCount="1037">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2264" uniqueCount="1055">
   <si>
     <t>LOCATIONS IN 1840s</t>
   </si>
@@ -2271,9 +2271,6 @@
     <t>TIRRIL</t>
   </si>
   <si>
-    <t>Swansea , 50 Winch Street</t>
-  </si>
-  <si>
     <t>18</t>
   </si>
   <si>
@@ -3259,6 +3256,63 @@
   </si>
   <si>
     <t>RR196</t>
+  </si>
+  <si>
+    <t>5545/8</t>
+  </si>
+  <si>
+    <t>RR207</t>
+  </si>
+  <si>
+    <t>RR208</t>
+  </si>
+  <si>
+    <t>RR209</t>
+  </si>
+  <si>
+    <t>RR210</t>
+  </si>
+  <si>
+    <t>RR212</t>
+  </si>
+  <si>
+    <t>RR217</t>
+  </si>
+  <si>
+    <t>RR213</t>
+  </si>
+  <si>
+    <t>RR219</t>
+  </si>
+  <si>
+    <t>RR220</t>
+  </si>
+  <si>
+    <t>RR223</t>
+  </si>
+  <si>
+    <t>RR226</t>
+  </si>
+  <si>
+    <t>Swansea , 50 Wind Street</t>
+  </si>
+  <si>
+    <t>RR228</t>
+  </si>
+  <si>
+    <t>RR229</t>
+  </si>
+  <si>
+    <t>RR232</t>
+  </si>
+  <si>
+    <t>3391</t>
+  </si>
+  <si>
+    <t>RR236</t>
+  </si>
+  <si>
+    <t>RR238</t>
   </si>
 </sst>
 </file>
@@ -3932,8 +3986,8 @@
   <dimension ref="A1:AA1006"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A388" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H420" sqref="H420"/>
+      <pane ySplit="6" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -4509,7 +4563,7 @@
         <v>31</v>
       </c>
       <c r="G26" s="82" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="I26" s="25"/>
     </row>
@@ -4621,7 +4675,12 @@
         <v>49</v>
       </c>
       <c r="E32" s="23"/>
-      <c r="G32" s="24"/>
+      <c r="F32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G32" s="82" t="s">
+        <v>1044</v>
+      </c>
       <c r="I32" s="25"/>
     </row>
     <row r="33" spans="1:10" ht="15.75" customHeight="1">
@@ -4636,7 +4695,12 @@
         <v>50</v>
       </c>
       <c r="E33" s="23"/>
-      <c r="G33" s="24"/>
+      <c r="F33" t="s">
+        <v>31</v>
+      </c>
+      <c r="G33" s="82" t="s">
+        <v>1044</v>
+      </c>
       <c r="I33" s="25"/>
     </row>
     <row r="34" spans="1:10" ht="15.75" customHeight="1">
@@ -4666,7 +4730,12 @@
         <v>52</v>
       </c>
       <c r="E35" s="23"/>
-      <c r="G35" s="24"/>
+      <c r="F35" s="74" t="s">
+        <v>31</v>
+      </c>
+      <c r="G35" s="82" t="s">
+        <v>1054</v>
+      </c>
       <c r="I35" s="25"/>
     </row>
     <row r="36" spans="1:10" ht="15.75" customHeight="1">
@@ -5340,7 +5409,12 @@
         <v>108</v>
       </c>
       <c r="E72" s="23"/>
-      <c r="G72" s="24"/>
+      <c r="F72" t="s">
+        <v>31</v>
+      </c>
+      <c r="G72" s="82" t="s">
+        <v>1037</v>
+      </c>
       <c r="I72" s="25"/>
     </row>
     <row r="73" spans="1:10" ht="13">
@@ -5546,7 +5620,7 @@
         <v>122</v>
       </c>
       <c r="G83" s="82" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="H83" s="26" t="s">
         <v>123</v>
@@ -5575,7 +5649,7 @@
       </c>
       <c r="G84" s="24"/>
       <c r="H84" s="79" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="I84" s="25"/>
     </row>
@@ -6003,7 +6077,7 @@
         <v>136</v>
       </c>
       <c r="G105" s="82" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="H105" s="26" t="s">
         <v>162</v>
@@ -6232,7 +6306,12 @@
       <c r="E118" s="28" t="s">
         <v>181</v>
       </c>
-      <c r="G118" s="24"/>
+      <c r="F118" t="s">
+        <v>31</v>
+      </c>
+      <c r="G118" s="82" t="s">
+        <v>1051</v>
+      </c>
       <c r="I118" s="25"/>
     </row>
     <row r="119" spans="1:10" ht="13">
@@ -7284,7 +7363,7 @@
         <v>293</v>
       </c>
       <c r="D165" s="12" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="E165" s="28" t="s">
         <v>294</v>
@@ -7293,7 +7372,7 @@
         <v>31</v>
       </c>
       <c r="G165" s="82" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="I165" s="25"/>
     </row>
@@ -7397,7 +7476,9 @@
       <c r="F170" s="26" t="s">
         <v>296</v>
       </c>
-      <c r="G170" s="24"/>
+      <c r="G170" s="82" t="s">
+        <v>1047</v>
+      </c>
       <c r="I170" s="25"/>
       <c r="J170" s="26" t="s">
         <v>306</v>
@@ -8972,7 +9053,12 @@
         <v>483</v>
       </c>
       <c r="E241" s="23"/>
-      <c r="G241" s="24"/>
+      <c r="F241" s="79" t="s">
+        <v>31</v>
+      </c>
+      <c r="G241" s="82" t="s">
+        <v>1040</v>
+      </c>
       <c r="I241" s="25"/>
     </row>
     <row r="242" spans="1:10" ht="13">
@@ -9178,7 +9264,9 @@
       <c r="F250" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="G250" s="24"/>
+      <c r="G250" s="82" t="s">
+        <v>1041</v>
+      </c>
       <c r="H250" s="26" t="s">
         <v>501</v>
       </c>
@@ -10074,7 +10162,9 @@
       <c r="F292" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="G292" s="24"/>
+      <c r="G292" s="82" t="s">
+        <v>1042</v>
+      </c>
       <c r="H292" s="26" t="s">
         <v>578</v>
       </c>
@@ -10092,7 +10182,12 @@
         <v>579</v>
       </c>
       <c r="E293" s="23"/>
-      <c r="G293" s="24"/>
+      <c r="F293" t="s">
+        <v>31</v>
+      </c>
+      <c r="G293" s="82" t="s">
+        <v>1043</v>
+      </c>
       <c r="I293" s="25"/>
     </row>
     <row r="294" spans="1:10" ht="13">
@@ -10167,7 +10262,12 @@
         <v>587</v>
       </c>
       <c r="E297" s="23"/>
-      <c r="G297" s="24"/>
+      <c r="F297" t="s">
+        <v>31</v>
+      </c>
+      <c r="G297" s="82" t="s">
+        <v>1052</v>
+      </c>
       <c r="I297" s="25"/>
     </row>
     <row r="298" spans="1:10" ht="13">
@@ -10182,7 +10282,12 @@
         <v>588</v>
       </c>
       <c r="E298" s="23"/>
-      <c r="G298" s="24"/>
+      <c r="F298" t="s">
+        <v>31</v>
+      </c>
+      <c r="G298" s="82" t="s">
+        <v>1052</v>
+      </c>
       <c r="I298" s="25"/>
     </row>
     <row r="299" spans="1:10" ht="15">
@@ -10352,7 +10457,7 @@
         <v>31</v>
       </c>
       <c r="G306" s="82" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="I306" s="25"/>
     </row>
@@ -10548,7 +10653,7 @@
         <v>31</v>
       </c>
       <c r="G317" s="82" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="I317" s="25"/>
     </row>
@@ -10671,7 +10776,9 @@
       <c r="F324" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="G324" s="24"/>
+      <c r="G324" s="82" t="s">
+        <v>1046</v>
+      </c>
       <c r="H324" s="26" t="s">
         <v>626</v>
       </c>
@@ -11452,7 +11559,12 @@
         <v>690</v>
       </c>
       <c r="E363" s="23"/>
-      <c r="G363" s="24"/>
+      <c r="F363" t="s">
+        <v>31</v>
+      </c>
+      <c r="G363" s="82" t="s">
+        <v>1039</v>
+      </c>
       <c r="I363" s="25"/>
     </row>
     <row r="364" spans="1:10" ht="13">
@@ -11819,9 +11931,11 @@
       <c r="F382" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="G382" s="24"/>
-      <c r="H382" s="26" t="s">
-        <v>721</v>
+      <c r="G382" s="82" t="s">
+        <v>1049</v>
+      </c>
+      <c r="H382" s="79" t="s">
+        <v>1048</v>
       </c>
       <c r="I382" s="25"/>
     </row>
@@ -11833,10 +11947,10 @@
         <v>17</v>
       </c>
       <c r="C383" s="29" t="s">
+        <v>721</v>
+      </c>
+      <c r="D383" s="21" t="s">
         <v>722</v>
-      </c>
-      <c r="D383" s="21" t="s">
-        <v>723</v>
       </c>
       <c r="E383" s="23"/>
       <c r="G383" s="24"/>
@@ -11851,7 +11965,7 @@
       </c>
       <c r="C384" s="23"/>
       <c r="D384" s="21" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E384" s="23"/>
       <c r="G384" s="24"/>
@@ -11866,7 +11980,7 @@
       </c>
       <c r="C385" s="23"/>
       <c r="D385" s="21" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="E385" s="23"/>
       <c r="G385" s="24"/>
@@ -11891,7 +12005,7 @@
       </c>
       <c r="G386" s="24"/>
       <c r="H386" s="26" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="I386" s="25"/>
     </row>
@@ -11906,14 +12020,14 @@
         <v>334</v>
       </c>
       <c r="D387" s="21" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="E387" s="23"/>
       <c r="F387" s="26" t="s">
         <v>31</v>
       </c>
       <c r="G387" s="27" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="I387" s="25"/>
     </row>
@@ -11928,7 +12042,7 @@
         <v>534</v>
       </c>
       <c r="D388" s="21" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="E388" s="23"/>
       <c r="G388" s="24"/>
@@ -11942,10 +12056,10 @@
         <v>24</v>
       </c>
       <c r="C389" s="29" t="s">
+        <v>729</v>
+      </c>
+      <c r="D389" s="21" t="s">
         <v>730</v>
-      </c>
-      <c r="D389" s="21" t="s">
-        <v>731</v>
       </c>
       <c r="E389" s="23"/>
       <c r="F389" s="26" t="s">
@@ -11954,7 +12068,7 @@
       <c r="G389" s="24"/>
       <c r="I389" s="25"/>
       <c r="J389" s="26" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="390" spans="1:10" ht="13">
@@ -11976,7 +12090,7 @@
       </c>
       <c r="G390" s="24"/>
       <c r="H390" s="26" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="I390" s="25"/>
     </row>
@@ -11989,14 +12103,14 @@
       </c>
       <c r="C391" s="23"/>
       <c r="D391" s="21" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="E391" s="23"/>
       <c r="F391" s="26" t="s">
         <v>145</v>
       </c>
       <c r="G391" s="35" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="I391" s="25"/>
       <c r="J391" s="41" t="s">
@@ -12012,14 +12126,14 @@
       </c>
       <c r="C392" s="23"/>
       <c r="D392" s="21" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E392" s="23"/>
       <c r="F392" s="26" t="s">
         <v>145</v>
       </c>
       <c r="G392" s="57" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="I392" s="25"/>
       <c r="J392" s="41" t="s">
@@ -12034,10 +12148,10 @@
         <v>28</v>
       </c>
       <c r="C393" s="29" t="s">
+        <v>737</v>
+      </c>
+      <c r="D393" s="21" t="s">
         <v>738</v>
-      </c>
-      <c r="D393" s="21" t="s">
-        <v>739</v>
       </c>
       <c r="E393" s="23"/>
       <c r="G393" s="24"/>
@@ -12052,7 +12166,7 @@
       </c>
       <c r="C394" s="23"/>
       <c r="D394" s="21" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="E394" s="23"/>
       <c r="G394" s="24"/>
@@ -12067,7 +12181,7 @@
       </c>
       <c r="C395" s="23"/>
       <c r="D395" s="21" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E395" s="23"/>
       <c r="G395" s="24"/>
@@ -12084,7 +12198,7 @@
         <v>337</v>
       </c>
       <c r="D396" s="21" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E396" s="23"/>
       <c r="G396" s="24"/>
@@ -12092,14 +12206,14 @@
     </row>
     <row r="397" spans="1:10" ht="13">
       <c r="A397" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B397" s="22">
         <v>1</v>
       </c>
       <c r="C397" s="23"/>
       <c r="D397" s="21" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="E397" s="28" t="s">
         <v>177</v>
@@ -12108,60 +12222,60 @@
         <v>145</v>
       </c>
       <c r="G397" s="35" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="I397" s="25"/>
     </row>
     <row r="398" spans="1:10" ht="13">
       <c r="A398" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B398" s="22">
         <v>2</v>
       </c>
       <c r="C398" s="23"/>
       <c r="D398" s="21" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E398" s="23"/>
       <c r="F398" s="26" t="s">
         <v>145</v>
       </c>
       <c r="G398" s="35" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="I398" s="25"/>
     </row>
     <row r="399" spans="1:10" ht="13">
       <c r="A399" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B399" s="22">
         <v>3</v>
       </c>
       <c r="C399" s="29" t="s">
+        <v>746</v>
+      </c>
+      <c r="D399" s="21" t="s">
         <v>747</v>
-      </c>
-      <c r="D399" s="21" t="s">
-        <v>748</v>
       </c>
       <c r="E399" s="23"/>
       <c r="F399" s="26" t="s">
+        <v>748</v>
+      </c>
+      <c r="G399" s="27" t="s">
         <v>749</v>
       </c>
-      <c r="G399" s="27" t="s">
+      <c r="I399" s="30" t="s">
         <v>750</v>
       </c>
-      <c r="I399" s="30" t="s">
+      <c r="J399" s="26" t="s">
         <v>751</v>
-      </c>
-      <c r="J399" s="26" t="s">
-        <v>752</v>
       </c>
     </row>
     <row r="400" spans="1:10" ht="15">
       <c r="A400" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B400" s="22">
         <v>4</v>
@@ -12170,7 +12284,7 @@
         <v>716</v>
       </c>
       <c r="D400" s="21" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="E400" s="23"/>
       <c r="F400" s="26" t="s">
@@ -12179,19 +12293,19 @@
       <c r="G400" s="24"/>
       <c r="I400" s="25"/>
       <c r="J400" s="52" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="401" spans="1:10" ht="13">
       <c r="A401" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B401" s="22">
         <v>5</v>
       </c>
       <c r="C401" s="23"/>
       <c r="D401" s="21" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="E401" s="28" t="s">
         <v>181</v>
@@ -12200,23 +12314,23 @@
         <v>145</v>
       </c>
       <c r="G401" s="35" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="I401" s="25"/>
       <c r="J401" s="26" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="402" spans="1:10" ht="13">
       <c r="A402" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B402" s="22">
         <v>6</v>
       </c>
       <c r="C402" s="23"/>
       <c r="D402" s="21" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="E402" s="23"/>
       <c r="G402" s="24"/>
@@ -12224,16 +12338,16 @@
     </row>
     <row r="403" spans="1:10" ht="13">
       <c r="A403" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B403" s="22">
         <v>7</v>
       </c>
       <c r="C403" s="29" t="s">
+        <v>758</v>
+      </c>
+      <c r="D403" s="21" t="s">
         <v>759</v>
-      </c>
-      <c r="D403" s="21" t="s">
-        <v>760</v>
       </c>
       <c r="E403" s="23"/>
       <c r="G403" s="24"/>
@@ -12241,7 +12355,7 @@
     </row>
     <row r="404" spans="1:10" ht="13">
       <c r="A404" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B404" s="22">
         <v>8</v>
@@ -12252,28 +12366,28 @@
       </c>
       <c r="E404" s="23"/>
       <c r="F404" s="26" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="G404" s="24"/>
       <c r="H404" s="51" t="s">
+        <v>760</v>
+      </c>
+      <c r="I404" s="59" t="s">
         <v>761</v>
       </c>
-      <c r="I404" s="59" t="s">
+      <c r="J404" s="26" t="s">
         <v>762</v>
-      </c>
-      <c r="J404" s="26" t="s">
-        <v>763</v>
       </c>
     </row>
     <row r="405" spans="1:10" ht="13">
       <c r="A405" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B405" s="22">
         <v>9</v>
       </c>
       <c r="C405" s="29" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="D405" s="21" t="s">
         <v>20</v>
@@ -12282,31 +12396,31 @@
         <v>95</v>
       </c>
       <c r="F405" s="26" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="G405" s="24"/>
       <c r="H405" s="60" t="s">
+        <v>764</v>
+      </c>
+      <c r="I405" s="59" t="s">
         <v>765</v>
       </c>
-      <c r="I405" s="59" t="s">
+      <c r="J405" s="26" t="s">
         <v>766</v>
-      </c>
-      <c r="J405" s="26" t="s">
-        <v>767</v>
       </c>
     </row>
     <row r="406" spans="1:10" ht="13">
       <c r="A406" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B406" s="22">
         <v>10</v>
       </c>
       <c r="C406" s="29" t="s">
+        <v>767</v>
+      </c>
+      <c r="D406" s="21" t="s">
         <v>768</v>
-      </c>
-      <c r="D406" s="21" t="s">
-        <v>769</v>
       </c>
       <c r="E406" s="23"/>
       <c r="G406" s="24"/>
@@ -12314,13 +12428,13 @@
     </row>
     <row r="407" spans="1:10" ht="13">
       <c r="A407" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B407" s="22">
         <v>11</v>
       </c>
       <c r="C407" s="29" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="D407" s="21" t="s">
         <v>20</v>
@@ -12331,22 +12445,22 @@
       </c>
       <c r="G407" s="24"/>
       <c r="H407" s="26" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="I407" s="25"/>
     </row>
     <row r="408" spans="1:10" ht="13">
       <c r="A408" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B408" s="22">
         <v>12</v>
       </c>
       <c r="C408" s="29" t="s">
+        <v>771</v>
+      </c>
+      <c r="D408" s="21" t="s">
         <v>772</v>
-      </c>
-      <c r="D408" s="21" t="s">
-        <v>773</v>
       </c>
       <c r="E408" s="23"/>
       <c r="G408" s="24"/>
@@ -12354,7 +12468,7 @@
     </row>
     <row r="409" spans="1:10" ht="15">
       <c r="A409" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B409" s="22">
         <v>13</v>
@@ -12369,13 +12483,13 @@
       </c>
       <c r="G409" s="24"/>
       <c r="H409" s="52" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="I409" s="25"/>
     </row>
     <row r="410" spans="1:10" ht="15">
       <c r="A410" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B410" s="22">
         <v>14</v>
@@ -12390,19 +12504,19 @@
       </c>
       <c r="G410" s="24"/>
       <c r="H410" s="52" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="I410" s="25"/>
     </row>
     <row r="411" spans="1:10" ht="15">
       <c r="A411" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B411" s="22">
         <v>15</v>
       </c>
       <c r="C411" s="29" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="D411" s="21" t="s">
         <v>20</v>
@@ -12413,13 +12527,13 @@
       </c>
       <c r="G411" s="24"/>
       <c r="H411" s="52" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="I411" s="25"/>
     </row>
     <row r="412" spans="1:10" ht="13">
       <c r="A412" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B412" s="22">
         <v>16</v>
@@ -12434,20 +12548,20 @@
       </c>
       <c r="G412" s="24"/>
       <c r="H412" s="51" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="I412" s="25"/>
     </row>
     <row r="413" spans="1:10" ht="13">
       <c r="A413" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B413" s="22">
         <v>17</v>
       </c>
       <c r="C413" s="23"/>
       <c r="D413" s="21" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="E413" s="23"/>
       <c r="G413" s="24"/>
@@ -12455,7 +12569,7 @@
     </row>
     <row r="414" spans="1:10" ht="15">
       <c r="A414" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B414" s="22">
         <v>18</v>
@@ -12469,23 +12583,23 @@
         <v>145</v>
       </c>
       <c r="G414" s="43" t="s">
+        <v>779</v>
+      </c>
+      <c r="H414" s="51" t="s">
         <v>780</v>
-      </c>
-      <c r="H414" s="51" t="s">
-        <v>781</v>
       </c>
       <c r="I414" s="25"/>
     </row>
     <row r="415" spans="1:10" ht="13">
       <c r="A415" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B415" s="22">
         <v>19</v>
       </c>
       <c r="C415" s="23"/>
       <c r="D415" s="21" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="E415" s="23"/>
       <c r="G415" s="24"/>
@@ -12493,14 +12607,14 @@
     </row>
     <row r="416" spans="1:10" ht="13">
       <c r="A416" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B416" s="22">
         <v>20</v>
       </c>
       <c r="C416" s="23"/>
       <c r="D416" s="21" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="E416" s="23"/>
       <c r="F416" s="26" t="s">
@@ -12508,16 +12622,16 @@
       </c>
       <c r="G416" s="24"/>
       <c r="H416" s="26" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I416" s="25"/>
       <c r="J416" s="26" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="417" spans="1:10" ht="14">
       <c r="A417" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B417" s="22">
         <v>21</v>
@@ -12530,45 +12644,45 @@
       </c>
       <c r="E417" s="23"/>
       <c r="F417" s="26" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="G417" s="24"/>
       <c r="H417" s="61" t="s">
+        <v>785</v>
+      </c>
+      <c r="I417" s="59" t="s">
         <v>786</v>
       </c>
-      <c r="I417" s="59" t="s">
+      <c r="J417" s="26" t="s">
         <v>787</v>
-      </c>
-      <c r="J417" s="26" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="418" spans="1:10" ht="15">
       <c r="A418" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B418" s="22">
         <v>22</v>
       </c>
       <c r="C418" s="29" t="s">
+        <v>788</v>
+      </c>
+      <c r="D418" s="21" t="s">
         <v>789</v>
-      </c>
-      <c r="D418" s="21" t="s">
-        <v>790</v>
       </c>
       <c r="E418" s="23"/>
       <c r="F418" s="26" t="s">
         <v>145</v>
       </c>
       <c r="G418" s="43" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="H418" s="62"/>
       <c r="I418" s="25"/>
     </row>
     <row r="419" spans="1:10" ht="13">
       <c r="A419" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B419" s="22">
         <v>23</v>
@@ -12577,43 +12691,43 @@
         <v>84</v>
       </c>
       <c r="D419" s="21" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="E419" s="23"/>
       <c r="F419" s="26" t="s">
+        <v>792</v>
+      </c>
+      <c r="G419" s="82" t="s">
+        <v>1035</v>
+      </c>
+      <c r="I419" s="59" t="s">
         <v>793</v>
       </c>
-      <c r="G419" s="82" t="s">
-        <v>1036</v>
-      </c>
-      <c r="I419" s="59" t="s">
+      <c r="J419" s="26" t="s">
         <v>794</v>
-      </c>
-      <c r="J419" s="26" t="s">
-        <v>795</v>
       </c>
     </row>
     <row r="420" spans="1:10" ht="13">
       <c r="A420" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B420" s="22">
         <v>24</v>
       </c>
       <c r="C420" s="23"/>
       <c r="D420" s="21" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="E420" s="23"/>
       <c r="G420" s="24"/>
       <c r="I420" s="25"/>
       <c r="J420" s="26" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="421" spans="1:10" ht="13">
       <c r="A421" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B421" s="22">
         <v>25</v>
@@ -12628,23 +12742,23 @@
       </c>
       <c r="G421" s="24"/>
       <c r="H421" s="26" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="I421" s="25"/>
       <c r="J421" s="26" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="422" spans="1:10" ht="13">
       <c r="A422" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B422" s="22">
         <v>26</v>
       </c>
       <c r="C422" s="23"/>
       <c r="D422" s="21" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="E422" s="23"/>
       <c r="G422" s="24"/>
@@ -12652,14 +12766,14 @@
     </row>
     <row r="423" spans="1:10" ht="13">
       <c r="A423" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B423" s="22">
         <v>27</v>
       </c>
       <c r="C423" s="23"/>
       <c r="D423" s="21" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E423" s="23"/>
       <c r="G423" s="24"/>
@@ -12667,33 +12781,33 @@
     </row>
     <row r="424" spans="1:10" ht="13">
       <c r="A424" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B424" s="22">
         <v>28</v>
       </c>
       <c r="C424" s="23"/>
       <c r="D424" s="21" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E424" s="23"/>
       <c r="F424" s="26" t="s">
         <v>145</v>
       </c>
       <c r="G424" s="35" t="s">
+        <v>800</v>
+      </c>
+      <c r="H424" s="32" t="s">
         <v>801</v>
-      </c>
-      <c r="H424" s="32" t="s">
-        <v>802</v>
       </c>
       <c r="I424" s="25"/>
       <c r="J424" s="26" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="425" spans="1:10" ht="13">
       <c r="A425" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B425" s="22">
         <v>29</v>
@@ -12709,41 +12823,41 @@
         <v>145</v>
       </c>
       <c r="G425" s="35" t="s">
+        <v>803</v>
+      </c>
+      <c r="H425" s="51" t="s">
         <v>804</v>
-      </c>
-      <c r="H425" s="51" t="s">
-        <v>805</v>
       </c>
       <c r="I425" s="25"/>
     </row>
     <row r="426" spans="1:10" ht="13">
       <c r="A426" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B426" s="22">
         <v>30</v>
       </c>
       <c r="C426" s="29" t="s">
+        <v>805</v>
+      </c>
+      <c r="D426" s="21" t="s">
         <v>806</v>
-      </c>
-      <c r="D426" s="21" t="s">
-        <v>807</v>
       </c>
       <c r="E426" s="23"/>
       <c r="F426" s="26" t="s">
         <v>145</v>
       </c>
       <c r="G426" s="27" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="I426" s="25"/>
       <c r="J426" s="26" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="427" spans="1:10" ht="13">
       <c r="A427" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B427" s="22">
         <v>31</v>
@@ -12754,31 +12868,31 @@
       </c>
       <c r="E427" s="23"/>
       <c r="F427" s="26" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="G427" s="27" t="s">
+        <v>809</v>
+      </c>
+      <c r="H427" s="51" t="s">
         <v>810</v>
       </c>
-      <c r="H427" s="51" t="s">
+      <c r="I427" s="63" t="s">
         <v>811</v>
       </c>
-      <c r="I427" s="63" t="s">
+      <c r="J427" s="26" t="s">
         <v>812</v>
-      </c>
-      <c r="J427" s="26" t="s">
-        <v>813</v>
       </c>
     </row>
     <row r="428" spans="1:10" ht="13">
       <c r="A428" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B428" s="22">
         <v>32</v>
       </c>
       <c r="C428" s="23"/>
       <c r="D428" s="21" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E428" s="23"/>
       <c r="G428" s="24"/>
@@ -12786,23 +12900,23 @@
     </row>
     <row r="429" spans="1:10" ht="14">
       <c r="A429" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B429" s="22">
         <v>33</v>
       </c>
       <c r="C429" s="29" t="s">
+        <v>814</v>
+      </c>
+      <c r="D429" s="21" t="s">
         <v>815</v>
-      </c>
-      <c r="D429" s="21" t="s">
-        <v>816</v>
       </c>
       <c r="E429" s="23"/>
       <c r="F429" s="26" t="s">
         <v>145</v>
       </c>
       <c r="G429" s="64" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="I429" s="25"/>
       <c r="J429" s="26" t="s">
@@ -12811,13 +12925,13 @@
     </row>
     <row r="430" spans="1:10" ht="13">
       <c r="A430" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B430" s="22">
         <v>34</v>
       </c>
       <c r="C430" s="29" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="D430" s="21" t="s">
         <v>20</v>
@@ -12828,36 +12942,36 @@
       </c>
       <c r="G430" s="24"/>
       <c r="H430" s="51" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="I430" s="25"/>
     </row>
     <row r="431" spans="1:10" ht="13">
       <c r="A431" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B431" s="22">
         <v>35</v>
       </c>
       <c r="C431" s="29" t="s">
+        <v>819</v>
+      </c>
+      <c r="D431" s="21" t="s">
         <v>820</v>
-      </c>
-      <c r="D431" s="21" t="s">
-        <v>821</v>
       </c>
       <c r="E431" s="23"/>
       <c r="F431" s="26" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G431" s="55"/>
       <c r="I431" s="25"/>
       <c r="J431" s="26" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="432" spans="1:10" ht="15">
       <c r="A432" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B432" s="22">
         <v>36</v>
@@ -12871,10 +12985,10 @@
         <v>145</v>
       </c>
       <c r="G432" s="43" t="s">
+        <v>822</v>
+      </c>
+      <c r="H432" s="52" t="s">
         <v>823</v>
-      </c>
-      <c r="H432" s="52" t="s">
-        <v>824</v>
       </c>
       <c r="I432" s="52"/>
       <c r="J432" s="26" t="s">
@@ -12883,7 +12997,7 @@
     </row>
     <row r="433" spans="1:10" ht="13">
       <c r="A433" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B433" s="22">
         <v>37</v>
@@ -12897,10 +13011,10 @@
         <v>145</v>
       </c>
       <c r="G433" s="57" t="s">
+        <v>824</v>
+      </c>
+      <c r="H433" s="51" t="s">
         <v>825</v>
-      </c>
-      <c r="H433" s="51" t="s">
-        <v>826</v>
       </c>
       <c r="I433" s="25"/>
       <c r="J433" s="26" t="s">
@@ -12909,7 +13023,7 @@
     </row>
     <row r="434" spans="1:10" ht="13">
       <c r="A434" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B434" s="22">
         <v>38</v>
@@ -12924,22 +13038,22 @@
       </c>
       <c r="G434" s="24"/>
       <c r="H434" s="26" t="s">
+        <v>826</v>
+      </c>
+      <c r="I434" s="30" t="s">
         <v>827</v>
-      </c>
-      <c r="I434" s="30" t="s">
-        <v>828</v>
       </c>
     </row>
     <row r="435" spans="1:10" ht="13">
       <c r="A435" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B435" s="22">
         <v>39</v>
       </c>
       <c r="C435" s="23"/>
       <c r="D435" s="21" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="E435" s="23"/>
       <c r="G435" s="24"/>
@@ -12947,7 +13061,7 @@
     </row>
     <row r="436" spans="1:10" ht="13">
       <c r="A436" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B436" s="22">
         <v>40</v>
@@ -12962,43 +13076,48 @@
       </c>
       <c r="G436" s="24"/>
       <c r="H436" s="26" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="I436" s="25"/>
       <c r="J436" s="26" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="437" spans="1:10" ht="13">
       <c r="A437" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B437" s="22">
         <v>41</v>
       </c>
       <c r="C437" s="23"/>
       <c r="D437" s="21" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="E437" s="23"/>
-      <c r="G437" s="24"/>
+      <c r="F437" s="79" t="s">
+        <v>31</v>
+      </c>
+      <c r="G437" s="82" t="s">
+        <v>1036</v>
+      </c>
       <c r="I437" s="25"/>
       <c r="J437" s="26" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="438" spans="1:10" ht="13">
       <c r="A438" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B438" s="22">
         <v>42</v>
       </c>
       <c r="C438" s="29" t="s">
+        <v>833</v>
+      </c>
+      <c r="D438" s="21" t="s">
         <v>834</v>
-      </c>
-      <c r="D438" s="21" t="s">
-        <v>835</v>
       </c>
       <c r="E438" s="23"/>
       <c r="F438" s="26" t="s">
@@ -13006,16 +13125,16 @@
       </c>
       <c r="G438" s="24"/>
       <c r="H438" s="51" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="I438" s="25"/>
       <c r="J438" s="26" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="439" spans="1:10" ht="13">
       <c r="A439" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B439" s="22">
         <v>43</v>
@@ -13030,12 +13149,12 @@
       </c>
       <c r="G439" s="24"/>
       <c r="H439" s="26" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="440" spans="1:10" ht="13">
       <c r="A440" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B440" s="22">
         <v>44</v>
@@ -13048,22 +13167,22 @@
       </c>
       <c r="E440" s="23"/>
       <c r="F440" s="26" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="G440" s="24"/>
       <c r="H440" s="26" t="s">
+        <v>837</v>
+      </c>
+      <c r="I440" s="59" t="s">
         <v>838</v>
       </c>
-      <c r="I440" s="59" t="s">
+      <c r="J440" s="26" t="s">
         <v>839</v>
-      </c>
-      <c r="J440" s="26" t="s">
-        <v>840</v>
       </c>
     </row>
     <row r="441" spans="1:10" ht="14">
       <c r="A441" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B441" s="22">
         <v>45</v>
@@ -13080,16 +13199,16 @@
       </c>
       <c r="G441" s="24"/>
       <c r="H441" s="61" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="I441" s="25"/>
       <c r="J441" s="65" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="442" spans="1:10" ht="13">
       <c r="A442" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B442" s="22">
         <v>46</v>
@@ -13098,25 +13217,25 @@
         <v>368</v>
       </c>
       <c r="D442" s="21" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="E442" s="23"/>
       <c r="G442" s="24"/>
       <c r="I442" s="25"/>
       <c r="J442" s="26" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="443" spans="1:10" ht="13">
       <c r="A443" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B443" s="22">
         <v>47</v>
       </c>
       <c r="C443" s="23"/>
       <c r="D443" s="21" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="E443" s="23"/>
       <c r="G443" s="24"/>
@@ -13124,7 +13243,7 @@
     </row>
     <row r="444" spans="1:10" ht="13">
       <c r="A444" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B444" s="22">
         <v>48</v>
@@ -13133,7 +13252,7 @@
         <v>59</v>
       </c>
       <c r="D444" s="21" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="E444" s="23"/>
       <c r="G444" s="24"/>
@@ -13141,7 +13260,7 @@
     </row>
     <row r="445" spans="1:10" ht="13">
       <c r="A445" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B445" s="22">
         <v>49</v>
@@ -13150,7 +13269,7 @@
         <v>59</v>
       </c>
       <c r="D445" s="21" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="E445" s="23"/>
       <c r="G445" s="24"/>
@@ -13158,7 +13277,7 @@
     </row>
     <row r="446" spans="1:10" ht="13">
       <c r="A446" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B446" s="22">
         <v>50</v>
@@ -13167,7 +13286,7 @@
         <v>487</v>
       </c>
       <c r="D446" s="21" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="E446" s="23"/>
       <c r="G446" s="24"/>
@@ -13175,7 +13294,7 @@
     </row>
     <row r="447" spans="1:10" ht="13">
       <c r="A447" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B447" s="22">
         <v>51</v>
@@ -13184,20 +13303,20 @@
         <v>404</v>
       </c>
       <c r="D447" s="21" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="E447" s="23"/>
       <c r="F447" s="74" t="s">
         <v>31</v>
       </c>
       <c r="G447" s="82" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="I447" s="25"/>
     </row>
     <row r="448" spans="1:10" ht="13">
       <c r="A448" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B448" s="22">
         <v>52</v>
@@ -13206,27 +13325,27 @@
         <v>404</v>
       </c>
       <c r="D448" s="21" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="E448" s="23"/>
       <c r="F448" s="74" t="s">
         <v>31</v>
       </c>
       <c r="G448" s="82" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="I448" s="25"/>
     </row>
     <row r="449" spans="1:10" ht="13">
       <c r="A449" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B449" s="22">
         <v>53</v>
       </c>
       <c r="C449" s="23"/>
       <c r="D449" s="21" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="E449" s="23"/>
       <c r="G449" s="24"/>
@@ -13234,13 +13353,13 @@
     </row>
     <row r="450" spans="1:10" ht="13">
       <c r="A450" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B450" s="22">
         <v>54</v>
       </c>
       <c r="C450" s="29" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="D450" s="21" t="s">
         <v>20</v>
@@ -13250,23 +13369,23 @@
         <v>145</v>
       </c>
       <c r="G450" s="35" t="s">
+        <v>852</v>
+      </c>
+      <c r="H450" s="51" t="s">
         <v>853</v>
-      </c>
-      <c r="H450" s="51" t="s">
-        <v>854</v>
       </c>
       <c r="I450" s="25"/>
     </row>
     <row r="451" spans="1:10" ht="13">
       <c r="A451" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B451" s="22">
         <v>55</v>
       </c>
       <c r="C451" s="23"/>
       <c r="D451" s="21" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="E451" s="23"/>
       <c r="G451" s="24"/>
@@ -13274,7 +13393,7 @@
     </row>
     <row r="452" spans="1:10" ht="13">
       <c r="A452" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B452" s="22">
         <v>56</v>
@@ -13291,15 +13410,15 @@
       </c>
       <c r="G452" s="24"/>
       <c r="H452" s="26" t="s">
+        <v>854</v>
+      </c>
+      <c r="I452" s="30" t="s">
         <v>855</v>
-      </c>
-      <c r="I452" s="30" t="s">
-        <v>856</v>
       </c>
     </row>
     <row r="453" spans="1:10" ht="13">
       <c r="A453" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B453" s="22">
         <v>57</v>
@@ -13308,17 +13427,17 @@
         <v>97</v>
       </c>
       <c r="D453" s="21" t="s">
+        <v>856</v>
+      </c>
+      <c r="E453" s="28" t="s">
         <v>857</v>
-      </c>
-      <c r="E453" s="28" t="s">
-        <v>858</v>
       </c>
       <c r="G453" s="24"/>
       <c r="I453" s="25"/>
     </row>
     <row r="454" spans="1:10" ht="13">
       <c r="A454" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B454" s="22">
         <v>58</v>
@@ -13333,15 +13452,17 @@
       <c r="F454" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="G454" s="24"/>
+      <c r="G454" s="82" t="s">
+        <v>1053</v>
+      </c>
       <c r="H454" s="51" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="I454" s="25"/>
     </row>
     <row r="455" spans="1:10" ht="13">
       <c r="A455" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B455" s="22">
         <v>59</v>
@@ -13350,7 +13471,7 @@
         <v>582</v>
       </c>
       <c r="D455" s="21" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="E455" s="23"/>
       <c r="G455" s="24"/>
@@ -13358,7 +13479,7 @@
     </row>
     <row r="456" spans="1:10" ht="13">
       <c r="A456" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B456" s="22">
         <v>60</v>
@@ -13372,10 +13493,10 @@
         <v>31</v>
       </c>
       <c r="G456" s="66" t="s">
+        <v>860</v>
+      </c>
+      <c r="H456" s="62" t="s">
         <v>861</v>
-      </c>
-      <c r="H456" s="62" t="s">
-        <v>862</v>
       </c>
       <c r="I456" s="25"/>
       <c r="J456" s="41" t="s">
@@ -13384,14 +13505,14 @@
     </row>
     <row r="457" spans="1:10" ht="13">
       <c r="A457" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B457" s="22">
         <v>61</v>
       </c>
       <c r="C457" s="23"/>
       <c r="D457" s="21" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="E457" s="23"/>
       <c r="G457" s="24"/>
@@ -13399,14 +13520,14 @@
     </row>
     <row r="458" spans="1:10" ht="13">
       <c r="A458" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B458" s="22">
         <v>62</v>
       </c>
       <c r="C458" s="23"/>
       <c r="D458" s="21" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="E458" s="23"/>
       <c r="G458" s="24"/>
@@ -13414,7 +13535,7 @@
     </row>
     <row r="459" spans="1:10" ht="13">
       <c r="A459" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B459" s="22">
         <v>63</v>
@@ -13423,7 +13544,7 @@
         <v>34</v>
       </c>
       <c r="D459" s="21" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="E459" s="23"/>
       <c r="G459" s="24"/>
@@ -13431,13 +13552,13 @@
     </row>
     <row r="460" spans="1:10" ht="13">
       <c r="A460" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B460" s="22">
         <v>64</v>
       </c>
       <c r="C460" s="29" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="D460" s="21" t="s">
         <v>20</v>
@@ -13447,10 +13568,10 @@
         <v>145</v>
       </c>
       <c r="G460" s="57" t="s">
+        <v>863</v>
+      </c>
+      <c r="H460" s="51" t="s">
         <v>864</v>
-      </c>
-      <c r="H460" s="51" t="s">
-        <v>865</v>
       </c>
       <c r="I460" s="25"/>
       <c r="J460" s="41" t="s">
@@ -13459,13 +13580,13 @@
     </row>
     <row r="461" spans="1:10" ht="13">
       <c r="A461" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B461" s="22">
         <v>65</v>
       </c>
       <c r="C461" s="29" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="D461" s="21" t="s">
         <v>20</v>
@@ -13476,13 +13597,13 @@
       </c>
       <c r="G461" s="24"/>
       <c r="H461" s="26" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="I461" s="25"/>
     </row>
     <row r="462" spans="1:10" ht="13">
       <c r="A462" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B462" s="22">
         <v>66</v>
@@ -13499,23 +13620,23 @@
       </c>
       <c r="G462" s="24"/>
       <c r="H462" s="26" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="I462" s="25"/>
       <c r="J462" s="26"/>
     </row>
     <row r="463" spans="1:10" ht="13">
       <c r="A463" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B463" s="22">
         <v>67</v>
       </c>
       <c r="C463" s="29" t="s">
+        <v>868</v>
+      </c>
+      <c r="D463" s="21" t="s">
         <v>869</v>
-      </c>
-      <c r="D463" s="21" t="s">
-        <v>870</v>
       </c>
       <c r="E463" s="23"/>
       <c r="G463" s="24"/>
@@ -13523,44 +13644,44 @@
     </row>
     <row r="464" spans="1:10" ht="13">
       <c r="A464" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B464" s="22">
         <v>68</v>
       </c>
       <c r="C464" s="23"/>
       <c r="D464" s="21" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="E464" s="23"/>
       <c r="F464" s="79" t="s">
         <v>31</v>
       </c>
       <c r="G464" s="82" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="I464" s="25"/>
     </row>
     <row r="465" spans="1:10" ht="13">
       <c r="A465" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B465" s="22">
         <v>69</v>
       </c>
       <c r="C465" s="23"/>
       <c r="D465" s="21" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="E465" s="23"/>
       <c r="F465" s="26" t="s">
         <v>145</v>
       </c>
       <c r="G465" s="66" t="s">
+        <v>872</v>
+      </c>
+      <c r="H465" s="62" t="s">
         <v>873</v>
-      </c>
-      <c r="H465" s="62" t="s">
-        <v>874</v>
       </c>
       <c r="I465" s="25"/>
       <c r="J465" s="41" t="s">
@@ -13569,14 +13690,14 @@
     </row>
     <row r="466" spans="1:10" ht="13">
       <c r="A466" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B466" s="22">
         <v>70</v>
       </c>
       <c r="C466" s="23"/>
       <c r="D466" s="21" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="E466" s="23"/>
       <c r="G466" s="24"/>
@@ -13584,7 +13705,7 @@
     </row>
     <row r="467" spans="1:10" ht="13">
       <c r="A467" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B467" s="22">
         <v>71</v>
@@ -13598,10 +13719,10 @@
         <v>145</v>
       </c>
       <c r="G467" s="66" t="s">
+        <v>875</v>
+      </c>
+      <c r="H467" s="62" t="s">
         <v>876</v>
-      </c>
-      <c r="H467" s="62" t="s">
-        <v>877</v>
       </c>
       <c r="I467" s="25"/>
       <c r="J467" s="41" t="s">
@@ -13610,24 +13731,24 @@
     </row>
     <row r="468" spans="1:10" ht="15">
       <c r="A468" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B468" s="22">
         <v>72</v>
       </c>
       <c r="C468" s="23"/>
       <c r="D468" s="21" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="E468" s="23"/>
       <c r="F468" s="26" t="s">
         <v>145</v>
       </c>
       <c r="G468" s="43" t="s">
+        <v>878</v>
+      </c>
+      <c r="H468" s="52" t="s">
         <v>879</v>
-      </c>
-      <c r="H468" s="52" t="s">
-        <v>880</v>
       </c>
       <c r="I468" s="25"/>
       <c r="J468" s="41" t="s">
@@ -13636,7 +13757,7 @@
     </row>
     <row r="469" spans="1:10" ht="13">
       <c r="A469" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B469" s="22">
         <v>73</v>
@@ -13653,74 +13774,79 @@
       </c>
       <c r="G469" s="24"/>
       <c r="H469" s="51" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="I469" s="25"/>
     </row>
     <row r="470" spans="1:10" ht="13">
       <c r="A470" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B470" s="22">
         <v>74</v>
       </c>
       <c r="C470" s="29" t="s">
+        <v>881</v>
+      </c>
+      <c r="D470" s="21" t="s">
         <v>882</v>
       </c>
-      <c r="D470" s="21" t="s">
-        <v>883</v>
-      </c>
       <c r="E470" s="23"/>
-      <c r="G470" s="24"/>
+      <c r="F470" s="79" t="s">
+        <v>31</v>
+      </c>
+      <c r="G470" s="82" t="s">
+        <v>1050</v>
+      </c>
       <c r="I470" s="25"/>
     </row>
     <row r="471" spans="1:10" ht="13">
       <c r="A471" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B471" s="22">
         <v>75</v>
       </c>
       <c r="C471" s="23"/>
       <c r="D471" s="21" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="E471" s="23"/>
       <c r="F471" s="26" t="s">
         <v>145</v>
       </c>
       <c r="G471" s="67" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="H471" s="51"/>
       <c r="I471" s="25"/>
     </row>
     <row r="472" spans="1:10" ht="13">
       <c r="A472" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B472" s="22">
         <v>76</v>
       </c>
       <c r="C472" s="23"/>
       <c r="D472" s="21" t="s">
+        <v>885</v>
+      </c>
+      <c r="E472" s="28" t="s">
         <v>886</v>
-      </c>
-      <c r="E472" s="28" t="s">
-        <v>887</v>
       </c>
       <c r="F472" s="26" t="s">
         <v>145</v>
       </c>
       <c r="G472" s="67" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="H472" s="51"/>
       <c r="I472" s="25"/>
     </row>
     <row r="473" spans="1:10" ht="15">
       <c r="A473" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B473" s="22">
         <v>77</v>
@@ -13734,10 +13860,10 @@
         <v>145</v>
       </c>
       <c r="G473" s="43" t="s">
+        <v>888</v>
+      </c>
+      <c r="H473" s="52" t="s">
         <v>889</v>
-      </c>
-      <c r="H473" s="52" t="s">
-        <v>890</v>
       </c>
       <c r="I473" s="25"/>
       <c r="J473" s="41" t="s">
@@ -13746,14 +13872,14 @@
     </row>
     <row r="474" spans="1:10" ht="13">
       <c r="A474" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B474" s="22">
         <v>78</v>
       </c>
       <c r="C474" s="23"/>
       <c r="D474" s="21" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="E474" s="28" t="s">
         <v>40</v>
@@ -13762,10 +13888,10 @@
         <v>145</v>
       </c>
       <c r="G474" s="57" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="H474" s="51" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="I474" s="25"/>
       <c r="J474" s="41" t="s">
@@ -13774,31 +13900,31 @@
     </row>
     <row r="475" spans="1:10" ht="13">
       <c r="A475" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B475" s="22">
         <v>79</v>
       </c>
       <c r="C475" s="23"/>
       <c r="D475" s="21" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="E475" s="23"/>
       <c r="G475" s="27" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="I475" s="25"/>
     </row>
     <row r="476" spans="1:10" ht="13">
       <c r="A476" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B476" s="22">
         <v>80</v>
       </c>
       <c r="C476" s="23"/>
       <c r="D476" s="21" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="E476" s="28" t="s">
         <v>44</v>
@@ -13807,10 +13933,10 @@
         <v>145</v>
       </c>
       <c r="G476" s="57" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="H476" s="51" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="I476" s="25"/>
       <c r="J476" s="41" t="s">
@@ -13819,14 +13945,14 @@
     </row>
     <row r="477" spans="1:10" ht="13">
       <c r="A477" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B477" s="22">
         <v>81</v>
       </c>
       <c r="C477" s="23"/>
       <c r="D477" s="21" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E477" s="23"/>
       <c r="G477" s="24"/>
@@ -13834,7 +13960,7 @@
     </row>
     <row r="478" spans="1:10" ht="13">
       <c r="A478" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B478" s="22">
         <v>82</v>
@@ -13848,10 +13974,10 @@
         <v>145</v>
       </c>
       <c r="G478" s="57" t="s">
+        <v>897</v>
+      </c>
+      <c r="H478" s="51" t="s">
         <v>898</v>
-      </c>
-      <c r="H478" s="51" t="s">
-        <v>899</v>
       </c>
       <c r="I478" s="25"/>
       <c r="J478" s="41" t="s">
@@ -13860,7 +13986,7 @@
     </row>
     <row r="479" spans="1:10" ht="15">
       <c r="A479" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B479" s="22">
         <v>83</v>
@@ -13874,10 +14000,10 @@
         <v>145</v>
       </c>
       <c r="G479" s="43" t="s">
+        <v>899</v>
+      </c>
+      <c r="H479" s="52" t="s">
         <v>900</v>
-      </c>
-      <c r="H479" s="52" t="s">
-        <v>901</v>
       </c>
       <c r="I479" s="25"/>
       <c r="J479" s="41" t="s">
@@ -13886,7 +14012,7 @@
     </row>
     <row r="480" spans="1:10" ht="13">
       <c r="A480" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B480" s="22">
         <v>84</v>
@@ -13900,10 +14026,10 @@
         <v>145</v>
       </c>
       <c r="G480" s="57" t="s">
+        <v>901</v>
+      </c>
+      <c r="H480" s="62" t="s">
         <v>902</v>
-      </c>
-      <c r="H480" s="62" t="s">
-        <v>903</v>
       </c>
       <c r="I480" s="25"/>
       <c r="J480" s="41" t="s">
@@ -13912,7 +14038,7 @@
     </row>
     <row r="481" spans="1:10" ht="13">
       <c r="A481" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B481" s="22">
         <v>85</v>
@@ -13928,16 +14054,16 @@
         <v>145</v>
       </c>
       <c r="G481" s="68" t="s">
+        <v>903</v>
+      </c>
+      <c r="H481" s="51" t="s">
         <v>904</v>
-      </c>
-      <c r="H481" s="51" t="s">
-        <v>905</v>
       </c>
       <c r="I481" s="25"/>
     </row>
     <row r="482" spans="1:10" ht="13">
       <c r="A482" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B482" s="22">
         <v>86</v>
@@ -13951,10 +14077,10 @@
         <v>145</v>
       </c>
       <c r="G482" s="53" t="s">
+        <v>905</v>
+      </c>
+      <c r="H482" s="51" t="s">
         <v>906</v>
-      </c>
-      <c r="H482" s="51" t="s">
-        <v>907</v>
       </c>
       <c r="I482" s="25"/>
       <c r="J482" s="41" t="s">
@@ -13963,24 +14089,24 @@
     </row>
     <row r="483" spans="1:10" ht="15">
       <c r="A483" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B483" s="22">
         <v>87</v>
       </c>
       <c r="C483" s="23"/>
       <c r="D483" s="21" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="E483" s="23"/>
       <c r="F483" s="26" t="s">
         <v>145</v>
       </c>
       <c r="G483" s="54" t="s">
+        <v>908</v>
+      </c>
+      <c r="H483" s="52" t="s">
         <v>909</v>
-      </c>
-      <c r="H483" s="52" t="s">
-        <v>910</v>
       </c>
       <c r="I483" s="25"/>
       <c r="J483" s="26" t="s">
@@ -13989,29 +14115,29 @@
     </row>
     <row r="484" spans="1:10" ht="13">
       <c r="A484" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B484" s="22">
         <v>88</v>
       </c>
       <c r="C484" s="29" t="s">
+        <v>910</v>
+      </c>
+      <c r="D484" s="21" t="s">
         <v>911</v>
-      </c>
-      <c r="D484" s="21" t="s">
-        <v>912</v>
       </c>
       <c r="E484" s="23"/>
       <c r="F484" s="26" t="s">
         <v>31</v>
       </c>
       <c r="G484" s="27" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="I484" s="25"/>
     </row>
     <row r="485" spans="1:10" ht="13">
       <c r="A485" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B485" s="22">
         <v>89</v>
@@ -14020,7 +14146,7 @@
         <v>84</v>
       </c>
       <c r="D485" s="21" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="E485" s="23"/>
       <c r="G485" s="24"/>
@@ -14028,7 +14154,7 @@
     </row>
     <row r="486" spans="1:10" ht="13">
       <c r="A486" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B486" s="22">
         <v>90</v>
@@ -14037,7 +14163,7 @@
         <v>59</v>
       </c>
       <c r="D486" s="21" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="E486" s="23"/>
       <c r="G486" s="24"/>
@@ -14045,16 +14171,16 @@
     </row>
     <row r="487" spans="1:10" ht="13">
       <c r="A487" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B487" s="22">
         <v>91</v>
       </c>
       <c r="C487" s="29" t="s">
+        <v>915</v>
+      </c>
+      <c r="D487" s="21" t="s">
         <v>916</v>
-      </c>
-      <c r="D487" s="21" t="s">
-        <v>917</v>
       </c>
       <c r="E487" s="23"/>
       <c r="G487" s="24"/>
@@ -14062,60 +14188,60 @@
     </row>
     <row r="488" spans="1:10" ht="13">
       <c r="A488" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B488" s="22">
         <v>92</v>
       </c>
       <c r="C488" s="29" t="s">
+        <v>917</v>
+      </c>
+      <c r="D488" s="21" t="s">
         <v>918</v>
-      </c>
-      <c r="D488" s="21" t="s">
-        <v>919</v>
       </c>
       <c r="E488" s="23"/>
       <c r="F488" t="s">
         <v>31</v>
       </c>
       <c r="G488" s="82" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="I488" s="25"/>
     </row>
     <row r="489" spans="1:10" ht="13">
       <c r="A489" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B489" s="22">
         <v>93</v>
       </c>
       <c r="C489" s="29" t="s">
+        <v>919</v>
+      </c>
+      <c r="D489" s="21" t="s">
         <v>920</v>
-      </c>
-      <c r="D489" s="21" t="s">
-        <v>921</v>
       </c>
       <c r="E489" s="23"/>
       <c r="F489" s="26" t="s">
         <v>31</v>
       </c>
       <c r="G489" s="27" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="I489" s="25"/>
     </row>
     <row r="490" spans="1:10" ht="13">
       <c r="A490" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B490" s="22">
         <v>94</v>
       </c>
       <c r="C490" s="29" t="s">
+        <v>922</v>
+      </c>
+      <c r="D490" s="21" t="s">
         <v>923</v>
-      </c>
-      <c r="D490" s="21" t="s">
-        <v>924</v>
       </c>
       <c r="E490" s="23"/>
       <c r="G490" s="24"/>
@@ -14123,16 +14249,16 @@
     </row>
     <row r="491" spans="1:10" ht="13">
       <c r="A491" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B491" s="22">
         <v>95</v>
       </c>
       <c r="C491" s="29" t="s">
+        <v>924</v>
+      </c>
+      <c r="D491" s="21" t="s">
         <v>925</v>
-      </c>
-      <c r="D491" s="21" t="s">
-        <v>926</v>
       </c>
       <c r="E491" s="23"/>
       <c r="G491" s="24"/>
@@ -14140,14 +14266,14 @@
     </row>
     <row r="492" spans="1:10" ht="13">
       <c r="A492" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B492" s="22">
         <v>96</v>
       </c>
       <c r="C492" s="23"/>
       <c r="D492" s="21" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="E492" s="23"/>
       <c r="G492" s="24"/>
@@ -14155,30 +14281,30 @@
     </row>
     <row r="493" spans="1:10" ht="13">
       <c r="A493" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B493" s="22">
         <v>97</v>
       </c>
       <c r="C493" s="23"/>
       <c r="D493" s="21" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="E493" s="23"/>
       <c r="F493" s="26" t="s">
         <v>145</v>
       </c>
       <c r="G493" s="53" t="s">
+        <v>928</v>
+      </c>
+      <c r="H493" s="51" t="s">
         <v>929</v>
-      </c>
-      <c r="H493" s="51" t="s">
-        <v>930</v>
       </c>
       <c r="I493" s="25"/>
     </row>
     <row r="494" spans="1:10" ht="13">
       <c r="A494" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B494" s="22">
         <v>98</v>
@@ -14187,23 +14313,23 @@
         <v>34</v>
       </c>
       <c r="D494" s="21" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="E494" s="23"/>
       <c r="F494" s="26" t="s">
         <v>145</v>
       </c>
       <c r="G494" s="57" t="s">
+        <v>931</v>
+      </c>
+      <c r="H494" s="62" t="s">
         <v>932</v>
-      </c>
-      <c r="H494" s="62" t="s">
-        <v>933</v>
       </c>
       <c r="I494" s="25"/>
     </row>
     <row r="495" spans="1:10" ht="15">
       <c r="A495" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B495" s="22">
         <v>99</v>
@@ -14217,16 +14343,16 @@
         <v>145</v>
       </c>
       <c r="G495" s="54" t="s">
+        <v>933</v>
+      </c>
+      <c r="H495" s="52" t="s">
         <v>934</v>
-      </c>
-      <c r="H495" s="52" t="s">
-        <v>935</v>
       </c>
       <c r="I495" s="25"/>
     </row>
     <row r="496" spans="1:10" ht="13">
       <c r="A496" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B496" s="22">
         <v>100</v>
@@ -14240,32 +14366,32 @@
         <v>145</v>
       </c>
       <c r="G496" s="66" t="s">
+        <v>935</v>
+      </c>
+      <c r="H496" s="26" t="s">
         <v>936</v>
-      </c>
-      <c r="H496" s="26" t="s">
-        <v>937</v>
       </c>
       <c r="I496" s="25"/>
     </row>
     <row r="497" spans="1:10" ht="13">
       <c r="A497" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B497" s="22">
         <v>101</v>
       </c>
       <c r="C497" s="23"/>
       <c r="D497" s="21" t="s">
+        <v>937</v>
+      </c>
+      <c r="E497" s="28" t="s">
         <v>938</v>
-      </c>
-      <c r="E497" s="28" t="s">
-        <v>939</v>
       </c>
       <c r="F497" s="26" t="s">
         <v>145</v>
       </c>
       <c r="G497" s="53" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="H497" s="51"/>
       <c r="I497" s="25"/>
@@ -14273,16 +14399,16 @@
     </row>
     <row r="498" spans="1:10" ht="13">
       <c r="A498" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B498" s="22">
         <v>102</v>
       </c>
       <c r="C498" s="29" t="s">
+        <v>940</v>
+      </c>
+      <c r="D498" s="21" t="s">
         <v>941</v>
-      </c>
-      <c r="D498" s="21" t="s">
-        <v>942</v>
       </c>
       <c r="E498" s="23"/>
       <c r="G498" s="24"/>
@@ -14290,16 +14416,16 @@
     </row>
     <row r="499" spans="1:10" ht="13">
       <c r="A499" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B499" s="22">
         <v>103</v>
       </c>
       <c r="C499" s="29" t="s">
+        <v>942</v>
+      </c>
+      <c r="D499" s="21" t="s">
         <v>943</v>
-      </c>
-      <c r="D499" s="21" t="s">
-        <v>944</v>
       </c>
       <c r="E499" s="23"/>
       <c r="G499" s="24"/>
@@ -14307,7 +14433,7 @@
     </row>
     <row r="500" spans="1:10" ht="13">
       <c r="A500" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B500" s="22">
         <v>104</v>
@@ -14324,13 +14450,13 @@
       </c>
       <c r="G500" s="24"/>
       <c r="H500" s="26" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="I500" s="25"/>
     </row>
     <row r="501" spans="1:10" ht="13">
       <c r="A501" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B501" s="22">
         <v>105</v>
@@ -14341,22 +14467,22 @@
       </c>
       <c r="E501" s="23"/>
       <c r="F501" s="26" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="G501" s="24"/>
       <c r="H501" s="26" t="s">
+        <v>945</v>
+      </c>
+      <c r="I501" s="30" t="s">
         <v>946</v>
       </c>
-      <c r="I501" s="30" t="s">
+      <c r="J501" s="26" t="s">
         <v>947</v>
-      </c>
-      <c r="J501" s="26" t="s">
-        <v>948</v>
       </c>
     </row>
     <row r="502" spans="1:10" ht="13">
       <c r="A502" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B502" s="22">
         <v>106</v>
@@ -14365,71 +14491,71 @@
         <v>97</v>
       </c>
       <c r="D502" s="21" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="E502" s="23"/>
       <c r="F502" s="26" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G502" s="55" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="I502" s="25"/>
       <c r="J502" s="69" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="503" spans="1:10" ht="13">
       <c r="A503" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B503" s="22">
         <v>107</v>
       </c>
       <c r="C503" s="29" t="s">
+        <v>951</v>
+      </c>
+      <c r="D503" s="21" t="s">
         <v>952</v>
-      </c>
-      <c r="D503" s="21" t="s">
-        <v>953</v>
       </c>
       <c r="E503" s="23"/>
       <c r="F503" s="26" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G503" s="24"/>
       <c r="I503" s="70" t="s">
+        <v>953</v>
+      </c>
+      <c r="J503" s="71" t="s">
         <v>954</v>
-      </c>
-      <c r="J503" s="71" t="s">
-        <v>955</v>
       </c>
     </row>
     <row r="504" spans="1:10" ht="13">
       <c r="A504" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B504" s="22">
         <v>108</v>
       </c>
       <c r="C504" s="23"/>
       <c r="D504" s="21" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="E504" s="23"/>
       <c r="F504" s="26" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G504" s="24"/>
       <c r="I504" s="72" t="s">
+        <v>956</v>
+      </c>
+      <c r="J504" s="6" t="s">
         <v>957</v>
-      </c>
-      <c r="J504" s="6" t="s">
-        <v>958</v>
       </c>
     </row>
     <row r="505" spans="1:10" ht="13">
       <c r="A505" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B505" s="22">
         <v>109</v>
@@ -14442,28 +14568,28 @@
       </c>
       <c r="E505" s="23"/>
       <c r="F505" s="26" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="G505" s="24"/>
       <c r="H505" s="26" t="s">
+        <v>958</v>
+      </c>
+      <c r="I505" s="70" t="s">
         <v>959</v>
       </c>
-      <c r="I505" s="70" t="s">
+      <c r="J505" s="26" t="s">
         <v>960</v>
-      </c>
-      <c r="J505" s="26" t="s">
-        <v>961</v>
       </c>
     </row>
     <row r="506" spans="1:10" ht="13">
       <c r="A506" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B506" s="22">
         <v>110</v>
       </c>
       <c r="C506" s="29" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="D506" s="21" t="s">
         <v>20</v>
@@ -14473,16 +14599,16 @@
         <v>145</v>
       </c>
       <c r="G506" s="27" t="s">
+        <v>962</v>
+      </c>
+      <c r="H506" s="26" t="s">
         <v>963</v>
-      </c>
-      <c r="H506" s="26" t="s">
-        <v>964</v>
       </c>
       <c r="I506" s="25"/>
     </row>
     <row r="507" spans="1:10" ht="13">
       <c r="A507" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B507" s="22">
         <v>111</v>
@@ -14495,22 +14621,22 @@
       </c>
       <c r="E507" s="23"/>
       <c r="F507" s="26" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="G507" s="24"/>
       <c r="H507" s="26" t="s">
+        <v>964</v>
+      </c>
+      <c r="I507" s="73" t="s">
         <v>965</v>
       </c>
-      <c r="I507" s="73" t="s">
+      <c r="J507" s="74" t="s">
         <v>966</v>
-      </c>
-      <c r="J507" s="74" t="s">
-        <v>967</v>
       </c>
     </row>
     <row r="508" spans="1:10" ht="13">
       <c r="A508" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B508" s="22">
         <v>112</v>
@@ -14519,23 +14645,23 @@
         <v>34</v>
       </c>
       <c r="D508" s="21" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="E508" s="23"/>
       <c r="F508" s="26" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G508" s="75" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="I508" s="25"/>
       <c r="J508" s="26" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="509" spans="1:10" ht="13">
       <c r="A509" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B509" s="22">
         <v>113</v>
@@ -14546,43 +14672,43 @@
       </c>
       <c r="E509" s="23"/>
       <c r="F509" s="26" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="G509" s="24"/>
       <c r="H509" s="26" t="s">
+        <v>971</v>
+      </c>
+      <c r="I509" s="73" t="s">
         <v>972</v>
       </c>
-      <c r="I509" s="73" t="s">
+      <c r="J509" s="74" t="s">
         <v>973</v>
-      </c>
-      <c r="J509" s="74" t="s">
-        <v>974</v>
       </c>
     </row>
     <row r="510" spans="1:10" ht="13">
       <c r="A510" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B510" s="22">
         <v>114</v>
       </c>
       <c r="C510" s="23"/>
       <c r="D510" s="21" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="E510" s="23"/>
       <c r="F510" s="26" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G510" s="24"/>
       <c r="I510" s="25"/>
       <c r="J510" s="26" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="511" spans="1:10" ht="13">
       <c r="A511" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B511" s="22">
         <v>115</v>
@@ -14597,13 +14723,13 @@
       </c>
       <c r="G511" s="24"/>
       <c r="H511" s="26" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="I511" s="25"/>
     </row>
     <row r="512" spans="1:10" ht="13">
       <c r="A512" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B512" s="22">
         <v>116</v>
@@ -14612,23 +14738,23 @@
         <v>348</v>
       </c>
       <c r="D512" s="21" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="E512" s="23"/>
       <c r="F512" s="26" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G512" s="24"/>
       <c r="I512" s="59" t="s">
+        <v>978</v>
+      </c>
+      <c r="J512" s="26" t="s">
         <v>979</v>
-      </c>
-      <c r="J512" s="26" t="s">
-        <v>980</v>
       </c>
     </row>
     <row r="513" spans="1:10" ht="13">
       <c r="A513" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B513" s="22">
         <v>117</v>
@@ -14639,22 +14765,22 @@
       </c>
       <c r="E513" s="23"/>
       <c r="F513" s="26" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="G513" s="24"/>
       <c r="H513" s="26" t="s">
+        <v>980</v>
+      </c>
+      <c r="I513" s="76" t="s">
         <v>981</v>
       </c>
-      <c r="I513" s="76" t="s">
+      <c r="J513" s="74" t="s">
         <v>982</v>
-      </c>
-      <c r="J513" s="74" t="s">
-        <v>983</v>
       </c>
     </row>
     <row r="514" spans="1:10" ht="13">
       <c r="A514" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B514" s="22">
         <v>118</v>
@@ -14665,22 +14791,22 @@
       </c>
       <c r="E514" s="23"/>
       <c r="F514" s="26" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="G514" s="24"/>
       <c r="H514" s="26" t="s">
+        <v>983</v>
+      </c>
+      <c r="I514" s="77" t="s">
         <v>984</v>
       </c>
-      <c r="I514" s="77" t="s">
+      <c r="J514" s="74" t="s">
         <v>985</v>
-      </c>
-      <c r="J514" s="74" t="s">
-        <v>986</v>
       </c>
     </row>
     <row r="515" spans="1:10" ht="13">
       <c r="A515" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B515" s="22">
         <v>119</v>
@@ -14691,45 +14817,47 @@
       </c>
       <c r="E515" s="23"/>
       <c r="F515" s="26" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="G515" s="24"/>
       <c r="H515" s="26" t="s">
+        <v>986</v>
+      </c>
+      <c r="I515" s="72" t="s">
         <v>987</v>
       </c>
-      <c r="I515" s="72" t="s">
+      <c r="J515" s="78" t="s">
         <v>988</v>
-      </c>
-      <c r="J515" s="78" t="s">
-        <v>989</v>
       </c>
     </row>
     <row r="516" spans="1:10" ht="13">
       <c r="A516" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B516" s="22">
         <v>120</v>
       </c>
       <c r="C516" s="23"/>
       <c r="D516" s="21" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="E516" s="23"/>
       <c r="F516" s="26" t="s">
+        <v>990</v>
+      </c>
+      <c r="G516" s="82" t="s">
+        <v>1038</v>
+      </c>
+      <c r="I516" s="41" t="s">
         <v>991</v>
       </c>
-      <c r="G516" s="24"/>
-      <c r="I516" s="41" t="s">
+      <c r="J516" s="79" t="s">
         <v>992</v>
-      </c>
-      <c r="J516" s="79" t="s">
-        <v>993</v>
       </c>
     </row>
     <row r="517" spans="1:10" ht="15">
       <c r="A517" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B517" s="22">
         <v>121</v>
@@ -14743,10 +14871,10 @@
         <v>145</v>
       </c>
       <c r="G517" s="43" t="s">
+        <v>993</v>
+      </c>
+      <c r="H517" s="52" t="s">
         <v>994</v>
-      </c>
-      <c r="H517" s="52" t="s">
-        <v>995</v>
       </c>
       <c r="I517" s="25"/>
       <c r="J517" s="41" t="s">
@@ -14755,24 +14883,24 @@
     </row>
     <row r="518" spans="1:10" ht="15">
       <c r="A518" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B518" s="22">
         <v>122</v>
       </c>
       <c r="C518" s="23"/>
       <c r="D518" s="21" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="E518" s="23"/>
       <c r="F518" s="26" t="s">
         <v>145</v>
       </c>
       <c r="G518" s="43" t="s">
+        <v>996</v>
+      </c>
+      <c r="H518" s="61" t="s">
         <v>997</v>
-      </c>
-      <c r="H518" s="61" t="s">
-        <v>998</v>
       </c>
       <c r="I518" s="25"/>
       <c r="J518" s="41" t="s">
@@ -14781,7 +14909,7 @@
     </row>
     <row r="519" spans="1:10" ht="13">
       <c r="A519" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B519" s="22">
         <v>123</v>
@@ -14795,17 +14923,17 @@
         <v>145</v>
       </c>
       <c r="G519" s="57" t="s">
+        <v>998</v>
+      </c>
+      <c r="H519" s="51" t="s">
         <v>999</v>
-      </c>
-      <c r="H519" s="51" t="s">
-        <v>1000</v>
       </c>
       <c r="I519" s="25"/>
       <c r="J519" s="41"/>
     </row>
     <row r="520" spans="1:10" ht="13">
       <c r="A520" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B520" s="22">
         <v>124</v>
@@ -14821,16 +14949,16 @@
         <v>145</v>
       </c>
       <c r="G520" s="27" t="s">
+        <v>1000</v>
+      </c>
+      <c r="H520" s="26" t="s">
         <v>1001</v>
-      </c>
-      <c r="H520" s="26" t="s">
-        <v>1002</v>
       </c>
       <c r="I520" s="25"/>
     </row>
     <row r="521" spans="1:10" ht="13">
       <c r="A521" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B521" s="22">
         <v>125</v>
@@ -14845,13 +14973,13 @@
       </c>
       <c r="G521" s="24"/>
       <c r="H521" s="26" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="I521" s="25"/>
     </row>
     <row r="522" spans="1:10" ht="13">
       <c r="A522" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B522" s="22">
         <v>126</v>
@@ -14867,78 +14995,80 @@
         <v>145</v>
       </c>
       <c r="G522" s="27" t="s">
+        <v>1003</v>
+      </c>
+      <c r="H522" s="26" t="s">
         <v>1004</v>
-      </c>
-      <c r="H522" s="26" t="s">
-        <v>1005</v>
       </c>
       <c r="I522" s="25"/>
     </row>
     <row r="523" spans="1:10" ht="13">
       <c r="A523" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B523" s="22">
         <v>127</v>
       </c>
       <c r="C523" s="29" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="D523" s="21" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="E523" s="23"/>
       <c r="F523" s="26" t="s">
-        <v>793</v>
-      </c>
-      <c r="G523" s="24"/>
+        <v>792</v>
+      </c>
+      <c r="G523" s="82" t="s">
+        <v>1045</v>
+      </c>
       <c r="I523" s="25"/>
       <c r="J523" s="69" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="524" spans="1:10" ht="13">
       <c r="A524" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B524" s="22">
         <v>128</v>
       </c>
       <c r="C524" s="29" t="s">
+        <v>1007</v>
+      </c>
+      <c r="D524" s="21" t="s">
         <v>1008</v>
-      </c>
-      <c r="D524" s="21" t="s">
-        <v>1009</v>
       </c>
       <c r="E524" s="23"/>
       <c r="F524" s="26" t="s">
         <v>145</v>
       </c>
       <c r="G524" s="35" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="I524" s="25"/>
       <c r="J524" s="26" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="525" spans="1:10" ht="13">
       <c r="A525" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B525" s="22">
         <v>129</v>
       </c>
       <c r="C525" s="23"/>
       <c r="D525" s="21" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="E525" s="23"/>
       <c r="F525" s="26" t="s">
         <v>145</v>
       </c>
       <c r="G525" s="35" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="I525" s="25"/>
       <c r="J525" s="41" t="s">
@@ -14947,7 +15077,7 @@
     </row>
     <row r="526" spans="1:10" ht="13">
       <c r="A526" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B526" s="22">
         <v>130</v>
@@ -14962,81 +15092,81 @@
       </c>
       <c r="G526" s="24"/>
       <c r="H526" s="26" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="I526" s="25"/>
     </row>
     <row r="527" spans="1:10" ht="13">
       <c r="A527" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B527" s="22">
         <v>131</v>
       </c>
       <c r="C527" s="29" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="D527" s="21" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="E527" s="23"/>
       <c r="F527" s="26" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G527" s="24"/>
       <c r="I527" s="30" t="s">
+        <v>1015</v>
+      </c>
+      <c r="J527" s="26" t="s">
         <v>1016</v>
-      </c>
-      <c r="J527" s="26" t="s">
-        <v>1017</v>
       </c>
     </row>
     <row r="528" spans="1:10" ht="13">
       <c r="A528" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B528" s="22">
         <v>132</v>
       </c>
       <c r="C528" s="23"/>
       <c r="D528" s="21" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="E528" s="23"/>
       <c r="F528" s="26" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G528" s="55" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="I528" s="25"/>
     </row>
     <row r="529" spans="1:10" ht="13">
       <c r="A529" s="21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B529" s="22">
         <v>133</v>
       </c>
       <c r="C529" s="29" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="D529" s="21" t="s">
         <v>20</v>
       </c>
       <c r="E529" s="23"/>
       <c r="F529" s="26" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="G529" s="80" t="s">
+        <v>1020</v>
+      </c>
+      <c r="H529" s="26" t="s">
         <v>1021</v>
-      </c>
-      <c r="H529" s="26" t="s">
-        <v>1022</v>
       </c>
       <c r="I529" s="25"/>
       <c r="J529" s="71" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="530" spans="1:10" ht="13">

</xml_diff>